<commit_message>
[이용섭] Add - [Storage/Image] 매대 캡쳐 이미지 9종 추가 Fixed - [Table] 테이블 기존 작업 개선 및 네이밍 변경(SaleStand -> StorageData)
</commit_message>
<xml_diff>
--- a/Content/TableData/Item.xlsx
+++ b/Content/TableData/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F235FF5-2961-4175-BDE3-715BFAB6FDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD9B11-D0D8-4FB9-9827-AA9E76376082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35460" yWindow="8100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>#</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -123,19 +123,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>캐시재화</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Gold</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Gold_Income</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 내에서 구할 수 있는 골드</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -516,7 +508,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A3" sqref="A3:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -537,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -567,7 +559,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -582,10 +574,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
         <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -639,6 +631,27 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>10000</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -648,10 +661,28 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
         <v>24</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>10000</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -662,10 +693,28 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[이용섭] Add - [ConstructItemElement] 마켓 확장 요소(Storage) 기능 추가.
</commit_message>
<xml_diff>
--- a/Content/TableData/Item.xlsx
+++ b/Content/TableData/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD9B11-D0D8-4FB9-9827-AA9E76376082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F7950D-1185-437B-AB84-6DFC0EE1F9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35460" yWindow="8100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43725" yWindow="5880" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J19"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>